<commit_message>
changed the HEX back to #
</commit_message>
<xml_diff>
--- a/Team05/Tests/iteration1/ResultQBasic1A-with-clause.xlsx
+++ b/Team05/Tests/iteration1/ResultQBasic1A-with-clause.xlsx
@@ -50,12 +50,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>stmtHEX</t>
-  </si>
-  <si>
-    <t>prog_lineHEX</t>
-  </si>
-  <si>
     <t>querystr</t>
   </si>
   <si>
@@ -143,66 +137,6 @@
     <t>constant c; Select BOOLEAN with c.value = 99999999999999</t>
   </si>
   <si>
-    <t>stmt s; Select s with s.stmtHEX = 17</t>
-  </si>
-  <si>
-    <t>stmt s; Select s with s.stmtHEX = 99999</t>
-  </si>
-  <si>
-    <t>stmt s; Select BOOLEAN with s.stmtHEX = 23</t>
-  </si>
-  <si>
-    <t>stmt s; Select BOOLEAN with s.stmtHEX = 999999</t>
-  </si>
-  <si>
-    <t>assign a; Select a with a.stmtHEX = 12</t>
-  </si>
-  <si>
-    <t>assign a; Select a with a.stmtHEX = 27</t>
-  </si>
-  <si>
-    <t>assign a; Select BOOLEAN with a.stmtHEX = 30</t>
-  </si>
-  <si>
-    <t>assign a; Select BOOLEAN with a.stmtHEX = 19</t>
-  </si>
-  <si>
-    <t>while w; Select w with w.stmtHEX = 19</t>
-  </si>
-  <si>
-    <t>while w; Select w with w.stmtHEX = 34</t>
-  </si>
-  <si>
-    <t>while w; Select BOOLEAN with w.stmtHEX = 8</t>
-  </si>
-  <si>
-    <t>while w; Select BOOLEAN with w.stmtHEX = 25</t>
-  </si>
-  <si>
-    <t>if i; Select i with i.stmtHEX = 38</t>
-  </si>
-  <si>
-    <t>if i; Select i with i.stmtHEX = 1</t>
-  </si>
-  <si>
-    <t>if i; Select BOOLEAN with i.stmtHEX = 38</t>
-  </si>
-  <si>
-    <t>if i; Select BOOLEAN with i.stmtHEX = 15</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select pl with pl.prog_lineHEX = 23</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select pl with pl.prog_lineHEX = 15081992</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select BOLLEAN with pl.prog_lineHEX = 1</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select BOOLEAN with pl.prog_lineHEX = 15081992</t>
-  </si>
-  <si>
     <t>procedure p; variable v; Select p with p.procName = v.varName</t>
   </si>
   <si>
@@ -240,6 +174,72 @@
   </si>
   <si>
     <t>1,10,11,12,13,14,15,16,18,19,2,20,21,22,23,24,25,26,27,28,29,3,30,31,32,33,34,35,36,37,38,39,4,40,5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>stmt#</t>
+  </si>
+  <si>
+    <t>prog_line#</t>
+  </si>
+  <si>
+    <t>stmt s; Select s with s.stmt# = 17</t>
+  </si>
+  <si>
+    <t>stmt s; Select s with s.stmt# = 99999</t>
+  </si>
+  <si>
+    <t>stmt s; Select BOOLEAN with s.stmt# = 23</t>
+  </si>
+  <si>
+    <t>stmt s; Select BOOLEAN with s.stmt# = 999999</t>
+  </si>
+  <si>
+    <t>assign a; Select a with a.stmt# = 12</t>
+  </si>
+  <si>
+    <t>assign a; Select a with a.stmt# = 27</t>
+  </si>
+  <si>
+    <t>assign a; Select BOOLEAN with a.stmt# = 30</t>
+  </si>
+  <si>
+    <t>assign a; Select BOOLEAN with a.stmt# = 19</t>
+  </si>
+  <si>
+    <t>while w; Select w with w.stmt# = 19</t>
+  </si>
+  <si>
+    <t>while w; Select w with w.stmt# = 34</t>
+  </si>
+  <si>
+    <t>while w; Select BOOLEAN with w.stmt# = 8</t>
+  </si>
+  <si>
+    <t>while w; Select BOOLEAN with w.stmt# = 25</t>
+  </si>
+  <si>
+    <t>if i; Select i with i.stmt# = 38</t>
+  </si>
+  <si>
+    <t>if i; Select i with i.stmt# = 1</t>
+  </si>
+  <si>
+    <t>if i; Select BOOLEAN with i.stmt# = 38</t>
+  </si>
+  <si>
+    <t>if i; Select BOOLEAN with i.stmt# = 15</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select pl with pl.prog_line# = 23</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select pl with pl.prog_line# = 15081992</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select BOLLEAN with pl.prog_line# = 1</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select BOOLEAN with pl.prog_line# = 15081992</t>
   </si>
 </sst>
 </file>
@@ -409,10 +409,10 @@
     <tableColumn id="9" uniqueName="value" name="value">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="stmtHEX" name="stmtHEX">
+    <tableColumn id="10" uniqueName="stmtHEX" name="stmt#">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@stmtHEX" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="prog_lineHEX" name="prog_lineHEX">
+    <tableColumn id="11" uniqueName="prog_lineHEX" name="prog_line#">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@prog_lineHEX" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="12" uniqueName="boolean" name="boolean3">
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -812,63 +812,63 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
-      </c>
-      <c r="X1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -878,17 +878,17 @@
       </c>
       <c r="F2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="P2">
         <v>12</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2">
@@ -909,13 +909,13 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -937,13 +937,13 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -956,22 +956,22 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P4">
         <v>11</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -991,13 +991,13 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1022,13 +1022,13 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1038,17 +1038,17 @@
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="P6">
         <v>11</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6">
@@ -1069,13 +1069,13 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1097,13 +1097,13 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -1116,22 +1116,22 @@
         <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P8">
         <v>11</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -1151,13 +1151,13 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -1170,17 +1170,17 @@
         <v>1</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P9">
         <v>4</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9">
@@ -1201,13 +1201,13 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1217,17 +1217,17 @@
         <v>1</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="P10">
         <v>11</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10">
@@ -1248,13 +1248,13 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1276,13 +1276,13 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -1295,22 +1295,22 @@
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P12">
         <v>11</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="S12">
         <v>1</v>
@@ -1330,13 +1330,13 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -1349,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1361,13 +1361,13 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -1377,20 +1377,20 @@
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="O14" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="P14">
         <v>14</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="S14">
         <v>1</v>
@@ -1410,13 +1410,13 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1426,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1438,13 +1438,13 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1454,22 +1454,22 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="P16">
         <v>14</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="S16">
         <v>1</v>
@@ -1489,13 +1489,13 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -1505,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1517,13 +1517,13 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1533,17 +1533,17 @@
         <v>1</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="P18">
         <v>3</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18">
@@ -1564,13 +1564,13 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1595,13 +1595,13 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <v>19</v>
@@ -1614,17 +1614,17 @@
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P20">
         <v>4</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20">
@@ -1645,13 +1645,13 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -1664,17 +1664,17 @@
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P21">
         <v>3</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21">
@@ -1695,13 +1695,13 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -1711,17 +1711,17 @@
         <v>1</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="P22">
         <v>3</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22">
@@ -1742,13 +1742,13 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23">
         <v>22</v>
@@ -1758,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1773,13 +1773,13 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24">
         <v>23</v>
@@ -1792,17 +1792,17 @@
         <v>1</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P24">
         <v>4</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24">
@@ -1823,13 +1823,13 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25">
         <v>24</v>
@@ -1842,17 +1842,17 @@
         <v>1</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P25">
         <v>3</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25">
@@ -1873,13 +1873,13 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -1889,17 +1889,17 @@
         <v>1</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="P26">
         <v>4</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26">
@@ -1920,13 +1920,13 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27">
         <v>26</v>
@@ -1936,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1951,13 +1951,13 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28">
         <v>27</v>
@@ -1970,17 +1970,17 @@
         <v>1</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P28">
         <v>4</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28">
@@ -2001,13 +2001,13 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29">
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D29">
         <v>28</v>
@@ -2020,17 +2020,17 @@
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P29">
         <v>3</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29">
@@ -2051,13 +2051,13 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30">
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30">
         <v>29</v>
@@ -2067,17 +2067,17 @@
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="P30">
         <v>3</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30">
@@ -2098,13 +2098,13 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31">
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31">
         <v>30</v>
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2129,13 +2129,13 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32">
         <v>31</v>
@@ -2148,17 +2148,17 @@
         <v>1</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="P32">
         <v>4</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32">
@@ -2179,13 +2179,13 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D33">
         <v>32</v>
@@ -2198,17 +2198,17 @@
         <v>1</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P33">
         <v>4</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33">
@@ -2229,13 +2229,13 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B34">
         <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34">
         <v>33</v>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>

</xml_diff>